<commit_message>
Revisi 7 by Fijay
</commit_message>
<xml_diff>
--- a/public/document/User Import.xlsx
+++ b/public/document/User Import.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FADB0011-6E5A-4FC5-8F58-F1AF798727A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -913,7 +914,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1009,7 +1010,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hipertaut" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
@@ -1318,11 +1319,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L112"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="B111" sqref="B111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3936,76 +3937,76 @@
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C44" r:id="rId2"/>
-    <hyperlink ref="C45" r:id="rId3"/>
-    <hyperlink ref="C46" r:id="rId4"/>
-    <hyperlink ref="C47" r:id="rId5"/>
-    <hyperlink ref="C48" r:id="rId6"/>
-    <hyperlink ref="C49" r:id="rId7"/>
-    <hyperlink ref="C50" r:id="rId8"/>
-    <hyperlink ref="C51" r:id="rId9"/>
-    <hyperlink ref="C52" r:id="rId10"/>
-    <hyperlink ref="C53" r:id="rId11"/>
-    <hyperlink ref="C54" r:id="rId12"/>
-    <hyperlink ref="C55" r:id="rId13"/>
-    <hyperlink ref="C56" r:id="rId14"/>
-    <hyperlink ref="C57" r:id="rId15"/>
-    <hyperlink ref="C112" r:id="rId16"/>
-    <hyperlink ref="C111" r:id="rId17"/>
-    <hyperlink ref="C110" r:id="rId18"/>
-    <hyperlink ref="C58" r:id="rId19"/>
-    <hyperlink ref="C59" r:id="rId20"/>
-    <hyperlink ref="C60" r:id="rId21"/>
-    <hyperlink ref="C61" r:id="rId22"/>
-    <hyperlink ref="C62" r:id="rId23"/>
-    <hyperlink ref="C63" r:id="rId24"/>
-    <hyperlink ref="C64" r:id="rId25"/>
-    <hyperlink ref="C65" r:id="rId26"/>
-    <hyperlink ref="C66" r:id="rId27"/>
-    <hyperlink ref="C67" r:id="rId28"/>
-    <hyperlink ref="C68" r:id="rId29"/>
-    <hyperlink ref="C69" r:id="rId30"/>
-    <hyperlink ref="C109" r:id="rId31"/>
-    <hyperlink ref="C108" r:id="rId32"/>
-    <hyperlink ref="C107" r:id="rId33"/>
-    <hyperlink ref="C106" r:id="rId34"/>
-    <hyperlink ref="C105" r:id="rId35"/>
-    <hyperlink ref="C104" r:id="rId36"/>
-    <hyperlink ref="C103" r:id="rId37"/>
-    <hyperlink ref="C70" r:id="rId38"/>
-    <hyperlink ref="C71" r:id="rId39"/>
-    <hyperlink ref="C72" r:id="rId40"/>
-    <hyperlink ref="C73" r:id="rId41"/>
-    <hyperlink ref="C74" r:id="rId42"/>
-    <hyperlink ref="C75" r:id="rId43"/>
-    <hyperlink ref="C76" r:id="rId44"/>
-    <hyperlink ref="C77" r:id="rId45"/>
-    <hyperlink ref="C78" r:id="rId46"/>
-    <hyperlink ref="C79" r:id="rId47"/>
-    <hyperlink ref="C80" r:id="rId48"/>
-    <hyperlink ref="C81" r:id="rId49"/>
-    <hyperlink ref="C82" r:id="rId50"/>
-    <hyperlink ref="C83" r:id="rId51"/>
-    <hyperlink ref="C84" r:id="rId52"/>
-    <hyperlink ref="C85" r:id="rId53"/>
-    <hyperlink ref="C86" r:id="rId54"/>
-    <hyperlink ref="C87" r:id="rId55"/>
-    <hyperlink ref="C88" r:id="rId56"/>
-    <hyperlink ref="C89" r:id="rId57"/>
-    <hyperlink ref="C90" r:id="rId58"/>
-    <hyperlink ref="C91" r:id="rId59"/>
-    <hyperlink ref="C92" r:id="rId60"/>
-    <hyperlink ref="C93" r:id="rId61"/>
-    <hyperlink ref="C94" r:id="rId62"/>
-    <hyperlink ref="C95" r:id="rId63"/>
-    <hyperlink ref="C96" r:id="rId64"/>
-    <hyperlink ref="C97" r:id="rId65"/>
-    <hyperlink ref="C98" r:id="rId66"/>
-    <hyperlink ref="C99" r:id="rId67"/>
-    <hyperlink ref="C100" r:id="rId68"/>
-    <hyperlink ref="C101" r:id="rId69"/>
-    <hyperlink ref="C102" r:id="rId70"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C44" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C45" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C46" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C47" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C48" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C49" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="C50" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="C51" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="C52" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="C53" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="C54" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="C55" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="C56" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="C57" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="C112" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="C111" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="C110" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="C58" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="C59" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="C60" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="C61" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="C62" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="C63" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="C64" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="C65" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="C66" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="C67" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="C68" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="C69" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="C109" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="C108" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="C107" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="C106" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="C105" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="C104" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="C103" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="C70" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="C71" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="C72" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="C73" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="C74" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="C75" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="C76" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="C77" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="C78" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="C79" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="C80" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="C81" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="C82" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="C83" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="C84" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="C85" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="C86" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="C87" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="C88" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="C89" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="C90" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="C91" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="C92" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="C93" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="C94" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="C95" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="C96" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="C97" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="C98" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="C99" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="C100" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="C101" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="C102" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId71"/>
@@ -4013,7 +4014,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4148,8 +4149,8 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1">
-    <sortState ref="A2:A25">
+  <autoFilter ref="A1" xr:uid="{00000000-0009-0000-0000-000001000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A25">
       <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>

</xml_diff>